<commit_message>
Some Imm & Imp ops
</commit_message>
<xml_diff>
--- a/opcodes.xlsx
+++ b/opcodes.xlsx
@@ -240,7 +240,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,13 +249,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="5"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
       <color theme="8"/>
       <name val="Calibri"/>
@@ -263,8 +257,10 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -279,7 +275,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -292,18 +289,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -622,7 +617,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,16 +691,16 @@
       <c r="G2">
         <v>4</v>
       </c>
-      <c r="H2" s="2">
-        <v>4</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="H2" s="1">
+        <v>4</v>
+      </c>
+      <c r="I2" s="1">
         <v>4</v>
       </c>
       <c r="K2">
         <v>6</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="1">
         <v>5</v>
       </c>
     </row>
@@ -713,7 +708,7 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>2</v>
       </c>
       <c r="D3">
@@ -725,16 +720,16 @@
       <c r="G3">
         <v>4</v>
       </c>
-      <c r="H3" s="2">
-        <v>4</v>
-      </c>
-      <c r="I3" s="2">
+      <c r="H3" s="1">
+        <v>4</v>
+      </c>
+      <c r="I3" s="1">
         <v>4</v>
       </c>
       <c r="K3">
         <v>6</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="1">
         <v>5</v>
       </c>
     </row>
@@ -742,7 +737,7 @@
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>2</v>
       </c>
       <c r="D4">
@@ -754,16 +749,16 @@
       <c r="G4">
         <v>4</v>
       </c>
-      <c r="H4" s="2">
-        <v>4</v>
-      </c>
-      <c r="I4" s="2">
+      <c r="H4" s="1">
+        <v>4</v>
+      </c>
+      <c r="I4" s="1">
         <v>4</v>
       </c>
       <c r="K4">
         <v>6</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="1">
         <v>5</v>
       </c>
     </row>
@@ -771,7 +766,7 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>2</v>
       </c>
       <c r="D5">
@@ -783,16 +778,16 @@
       <c r="G5">
         <v>4</v>
       </c>
-      <c r="H5" s="2">
-        <v>4</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="H5" s="1">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1">
         <v>4</v>
       </c>
       <c r="K5">
         <v>6</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="1">
         <v>5</v>
       </c>
     </row>
@@ -800,7 +795,7 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>2</v>
       </c>
       <c r="D6">
@@ -812,16 +807,16 @@
       <c r="G6">
         <v>4</v>
       </c>
-      <c r="H6" s="2">
-        <v>4</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1">
         <v>4</v>
       </c>
       <c r="K6">
         <v>6</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="1">
         <v>5</v>
       </c>
     </row>
@@ -829,7 +824,7 @@
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>2</v>
       </c>
       <c r="D8">
@@ -849,7 +844,7 @@
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>2</v>
       </c>
       <c r="D9">
@@ -869,7 +864,7 @@
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>2</v>
       </c>
       <c r="D10">
@@ -889,7 +884,7 @@
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>2</v>
       </c>
       <c r="D11">
@@ -926,7 +921,7 @@
       <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>2</v>
       </c>
     </row>
@@ -934,7 +929,7 @@
       <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>2</v>
       </c>
     </row>
@@ -959,7 +954,7 @@
       <c r="A17" t="s">
         <v>25</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>2</v>
       </c>
     </row>
@@ -967,7 +962,7 @@
       <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>2</v>
       </c>
     </row>
@@ -998,16 +993,16 @@
       <c r="G21">
         <v>4</v>
       </c>
-      <c r="H21" s="2">
-        <v>4</v>
-      </c>
-      <c r="I21" s="2">
+      <c r="H21" s="1">
+        <v>4</v>
+      </c>
+      <c r="I21" s="1">
         <v>4</v>
       </c>
       <c r="K21">
         <v>6</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L21" s="1">
         <v>5</v>
       </c>
     </row>
@@ -1043,7 +1038,7 @@
       <c r="A25" t="s">
         <v>31</v>
       </c>
-      <c r="M25" s="1">
+      <c r="M25" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1051,7 +1046,7 @@
       <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="M26" s="1">
+      <c r="M26" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1059,7 +1054,7 @@
       <c r="A27" t="s">
         <v>33</v>
       </c>
-      <c r="M27" s="1">
+      <c r="M27" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1067,7 +1062,7 @@
       <c r="A28" t="s">
         <v>34</v>
       </c>
-      <c r="M28" s="1">
+      <c r="M28" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1075,7 +1070,7 @@
       <c r="A29" t="s">
         <v>35</v>
       </c>
-      <c r="M29" s="1">
+      <c r="M29" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1083,7 +1078,7 @@
       <c r="A30" t="s">
         <v>36</v>
       </c>
-      <c r="M30" s="1">
+      <c r="M30" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1091,7 +1086,7 @@
       <c r="A31" t="s">
         <v>37</v>
       </c>
-      <c r="M31" s="1">
+      <c r="M31" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1099,7 +1094,7 @@
       <c r="A32" t="s">
         <v>38</v>
       </c>
-      <c r="M32" s="1">
+      <c r="M32" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1258,16 +1253,16 @@
       <c r="G54">
         <v>4</v>
       </c>
-      <c r="H54" s="2">
-        <v>4</v>
-      </c>
-      <c r="I54" s="2">
+      <c r="H54" s="1">
+        <v>4</v>
+      </c>
+      <c r="I54" s="1">
         <v>4</v>
       </c>
       <c r="K54">
         <v>6</v>
       </c>
-      <c r="L54" s="2">
+      <c r="L54" s="1">
         <v>5</v>
       </c>
     </row>
@@ -1287,7 +1282,7 @@
       <c r="G55">
         <v>4</v>
       </c>
-      <c r="I55" s="2">
+      <c r="I55" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1307,7 +1302,7 @@
       <c r="G56">
         <v>4</v>
       </c>
-      <c r="H56" s="2">
+      <c r="H56" s="1">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Status register bit set/clr operations
</commit_message>
<xml_diff>
--- a/opcodes.xlsx
+++ b/opcodes.xlsx
@@ -912,10 +912,10 @@
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="3">
         <v>2</v>
       </c>
     </row>
@@ -938,10 +938,10 @@
       <c r="H8">
         <v>7</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="3">
         <v>2</v>
       </c>
     </row>
@@ -964,10 +964,10 @@
       <c r="H9">
         <v>7</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="3">
         <v>2</v>
       </c>
     </row>
@@ -990,10 +990,10 @@
       <c r="H10">
         <v>7</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="O10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1016,18 +1016,18 @@
       <c r="H11">
         <v>7</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="O11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="O12" s="4" t="s">
+      <c r="O12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1047,10 +1047,10 @@
       <c r="H13">
         <v>7</v>
       </c>
-      <c r="O13" s="4" t="s">
+      <c r="O13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="3">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Using PLL to generate clocks, FSM now recognisible
</commit_message>
<xml_diff>
--- a/opcodes.xlsx
+++ b/opcodes.xlsx
@@ -263,18 +263,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -298,18 +292,115 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -644,7 +735,7 @@
     <col min="12" max="12" width="4.25" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="2.875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4.25" customWidth="1"/>
-    <col min="15" max="15" width="4.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.375" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="3.875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4.375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="3.625" bestFit="1" customWidth="1"/>
@@ -699,7 +790,7 @@
       <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>68</v>
       </c>
       <c r="P1" t="s">
@@ -743,7 +834,7 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2">
         <v>2</v>
       </c>
       <c r="D2">
@@ -752,7 +843,7 @@
       <c r="E2">
         <v>4</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2">
         <v>4</v>
       </c>
       <c r="H2" s="1">
@@ -767,10 +858,10 @@
       <c r="L2" s="1">
         <v>5</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="3">
+      <c r="U2">
         <v>3</v>
       </c>
       <c r="X2">
@@ -781,7 +872,7 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
@@ -790,7 +881,7 @@
       <c r="E3">
         <v>4</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3">
         <v>4</v>
       </c>
       <c r="H3" s="1">
@@ -805,7 +896,7 @@
       <c r="L3" s="1">
         <v>5</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>40</v>
       </c>
       <c r="U3">
@@ -816,7 +907,7 @@
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
@@ -825,7 +916,7 @@
       <c r="E4">
         <v>4</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4">
         <v>4</v>
       </c>
       <c r="H4" s="1">
@@ -840,7 +931,7 @@
       <c r="L4" s="1">
         <v>5</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="3" t="s">
         <v>41</v>
       </c>
       <c r="P4">
@@ -851,7 +942,7 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>2</v>
       </c>
       <c r="D5">
@@ -860,7 +951,7 @@
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5">
         <v>4</v>
       </c>
       <c r="H5" s="1">
@@ -875,7 +966,7 @@
       <c r="L5" s="1">
         <v>5</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="3" t="s">
         <v>42</v>
       </c>
       <c r="P5">
@@ -886,7 +977,7 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>2</v>
       </c>
       <c r="D6">
@@ -895,7 +986,7 @@
       <c r="E6">
         <v>4</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6">
         <v>4</v>
       </c>
       <c r="H6" s="1">
@@ -912,10 +1003,10 @@
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7">
         <v>2</v>
       </c>
     </row>
@@ -923,7 +1014,7 @@
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8">
         <v>2</v>
       </c>
       <c r="D8">
@@ -938,10 +1029,10 @@
       <c r="H8">
         <v>7</v>
       </c>
-      <c r="O8" s="5" t="s">
+      <c r="O8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8">
         <v>2</v>
       </c>
     </row>
@@ -949,7 +1040,7 @@
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>2</v>
       </c>
       <c r="D9">
@@ -964,10 +1055,10 @@
       <c r="H9">
         <v>7</v>
       </c>
-      <c r="O9" s="5" t="s">
+      <c r="O9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9">
         <v>2</v>
       </c>
     </row>
@@ -975,7 +1066,7 @@
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10">
         <v>2</v>
       </c>
       <c r="D10">
@@ -990,10 +1081,10 @@
       <c r="H10">
         <v>7</v>
       </c>
-      <c r="O10" s="5" t="s">
+      <c r="O10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10">
         <v>2</v>
       </c>
     </row>
@@ -1001,7 +1092,7 @@
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11">
         <v>2</v>
       </c>
       <c r="D11">
@@ -1016,18 +1107,18 @@
       <c r="H11">
         <v>7</v>
       </c>
-      <c r="O11" s="5" t="s">
+      <c r="O11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="P11" s="3">
+      <c r="P11">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="O12" s="5" t="s">
+      <c r="O12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="P12" s="3">
+      <c r="P12">
         <v>2</v>
       </c>
     </row>
@@ -1047,10 +1138,10 @@
       <c r="H13">
         <v>7</v>
       </c>
-      <c r="O13" s="5" t="s">
+      <c r="O13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P13" s="3">
+      <c r="P13">
         <v>2</v>
       </c>
     </row>
@@ -1058,7 +1149,7 @@
       <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14">
         <v>2</v>
       </c>
     </row>
@@ -1066,13 +1157,13 @@
       <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="3">
-        <v>2</v>
-      </c>
-      <c r="O15" s="5" t="s">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="O15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="P15" s="3">
+      <c r="P15">
         <v>2</v>
       </c>
     </row>
@@ -1092,10 +1183,10 @@
       <c r="H16">
         <v>7</v>
       </c>
-      <c r="O16" s="5" t="s">
+      <c r="O16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="P16" s="3">
+      <c r="P16">
         <v>2</v>
       </c>
     </row>
@@ -1103,13 +1194,13 @@
       <c r="A17" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="3">
-        <v>2</v>
-      </c>
-      <c r="O17" s="5" t="s">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="O17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="P17" s="3">
+      <c r="P17">
         <v>2</v>
       </c>
     </row>
@@ -1117,21 +1208,21 @@
       <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="3">
-        <v>2</v>
-      </c>
-      <c r="O18" s="5" t="s">
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="O18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="P18" s="3">
+      <c r="P18">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="O19" s="5" t="s">
+      <c r="O19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="P19" s="3">
+      <c r="P19">
         <v>2</v>
       </c>
     </row>
@@ -1145,10 +1236,10 @@
       <c r="G20">
         <v>4</v>
       </c>
-      <c r="O20" s="5" t="s">
+      <c r="O20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="P20" s="3">
+      <c r="P20">
         <v>2</v>
       </c>
     </row>
@@ -1194,10 +1285,10 @@
       <c r="G22">
         <v>4</v>
       </c>
-      <c r="O22" s="4" t="s">
+      <c r="O22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="Q22" s="3">
+      <c r="Q22">
         <v>2</v>
       </c>
       <c r="R22">
@@ -1206,7 +1297,7 @@
       <c r="S22">
         <v>4</v>
       </c>
-      <c r="U22" s="3">
+      <c r="U22">
         <v>4</v>
       </c>
       <c r="V22" s="1">
@@ -1235,10 +1326,10 @@
       <c r="G23">
         <v>4</v>
       </c>
-      <c r="O23" s="4" t="s">
+      <c r="O23" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="Q23" s="3">
+      <c r="Q23">
         <v>2</v>
       </c>
       <c r="R23">
@@ -1247,7 +1338,7 @@
       <c r="T23">
         <v>4</v>
       </c>
-      <c r="U23" s="3">
+      <c r="U23">
         <v>4</v>
       </c>
       <c r="W23" s="1">
@@ -1255,10 +1346,10 @@
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="O24" s="4" t="s">
+      <c r="O24" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="Q24" s="3">
+      <c r="Q24">
         <v>2</v>
       </c>
       <c r="R24">
@@ -1267,7 +1358,7 @@
       <c r="S24">
         <v>4</v>
       </c>
-      <c r="U24" s="3">
+      <c r="U24">
         <v>4</v>
       </c>
       <c r="V24" s="1">
@@ -1281,7 +1372,7 @@
       <c r="M25" s="2">
         <v>2</v>
       </c>
-      <c r="O25" s="4" t="s">
+      <c r="O25" s="3" t="s">
         <v>59</v>
       </c>
       <c r="R25">
@@ -1290,7 +1381,7 @@
       <c r="S25">
         <v>4</v>
       </c>
-      <c r="U25" s="3">
+      <c r="U25">
         <v>4</v>
       </c>
       <c r="V25">
@@ -1313,7 +1404,7 @@
       <c r="M26" s="2">
         <v>2</v>
       </c>
-      <c r="O26" s="4" t="s">
+      <c r="O26" s="3" t="s">
         <v>60</v>
       </c>
       <c r="R26">
@@ -1322,7 +1413,7 @@
       <c r="T26">
         <v>4</v>
       </c>
-      <c r="U26" s="3">
+      <c r="U26">
         <v>4</v>
       </c>
     </row>
@@ -1333,7 +1424,7 @@
       <c r="M27" s="2">
         <v>2</v>
       </c>
-      <c r="O27" s="4" t="s">
+      <c r="O27" s="3" t="s">
         <v>61</v>
       </c>
       <c r="R27">
@@ -1342,7 +1433,7 @@
       <c r="S27">
         <v>4</v>
       </c>
-      <c r="U27" s="3">
+      <c r="U27">
         <v>4</v>
       </c>
     </row>
@@ -1361,7 +1452,7 @@
       <c r="M29" s="2">
         <v>2</v>
       </c>
-      <c r="O29" s="4" t="s">
+      <c r="O29" s="3" t="s">
         <v>62</v>
       </c>
       <c r="P29">
@@ -1375,7 +1466,7 @@
       <c r="M30" s="2">
         <v>2</v>
       </c>
-      <c r="O30" s="4" t="s">
+      <c r="O30" s="3" t="s">
         <v>63</v>
       </c>
       <c r="P30">
@@ -1389,7 +1480,7 @@
       <c r="M31" s="2">
         <v>2</v>
       </c>
-      <c r="O31" s="4" t="s">
+      <c r="O31" s="3" t="s">
         <v>64</v>
       </c>
       <c r="P31">
@@ -1403,7 +1494,7 @@
       <c r="M32" s="2">
         <v>2</v>
       </c>
-      <c r="O32" s="4" t="s">
+      <c r="O32" s="3" t="s">
         <v>65</v>
       </c>
       <c r="P32">
@@ -1411,7 +1502,7 @@
       </c>
     </row>
     <row r="34" spans="15:27" x14ac:dyDescent="0.25">
-      <c r="O34" s="4" t="s">
+      <c r="O34" s="3" t="s">
         <v>66</v>
       </c>
       <c r="AA34">
@@ -1419,7 +1510,7 @@
       </c>
     </row>
     <row r="35" spans="15:27" x14ac:dyDescent="0.25">
-      <c r="O35" s="4" t="s">
+      <c r="O35" s="3" t="s">
         <v>67</v>
       </c>
       <c r="P35">
@@ -1427,6 +1518,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A7:M7 Q15:XFD20 O21:XFD21 O3:XFD6 A2:B6 H2:M6 O14:XFD14 Q7:XFD13 O28:XFD34 O22:P24 R22:T24 O25:T27 V22:XFD27 D2:F6 A12:M13 A8:A11 C8:M11 A16:M16 A14:A15 C14:M15 A19:M1048576 A17:A18 C17:M18 O2:T2 V2:XFD2 O36:XFD1048576 Q35:XFD35">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="1">
+      <formula>LEN(TRIM(A2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
CMP, CPX, CPY @ Imm, Abs
</commit_message>
<xml_diff>
--- a/opcodes.xlsx
+++ b/opcodes.xlsx
@@ -301,7 +301,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1518,8 +1532,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A7:M7 Q15:XFD20 O21:XFD21 O3:XFD6 A2:B6 H2:M6 O14:XFD14 Q7:XFD13 O28:XFD34 O22:P24 R22:T24 O25:T27 V22:XFD27 D2:F6 A12:M13 A8:A11 C8:M11 A16:M16 A14:A15 C14:M15 A19:M1048576 A17:A18 C17:M18 O2:T2 V2:XFD2 O36:XFD1048576 Q35:XFD35">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="1">
+  <conditionalFormatting sqref="A7:M7 Q15:XFD20 O21:XFD21 O3:XFD6 A2:B6 H2:M6 O14:XFD14 Q7:XFD13 O28:XFD34 O22:P24 R22:T24 O25:T27 V22:XFD27 D2:F6 A12:M13 A8:A11 C8:M11 A16:M16 A14:A15 C14:M15 A19:M19 A17:A18 C17:M18 O2:T2 V2:XFD2 O36:XFD1048576 Q35:XFD35 A24:M1048576 A21:B23 D21:F23 A20:F20 H20:M23">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ZpY addressing (1 cycle before spec)
</commit_message>
<xml_diff>
--- a/opcodes.xlsx
+++ b/opcodes.xlsx
@@ -308,7 +308,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1353,7 +1360,7 @@
       <c r="R23">
         <v>3</v>
       </c>
-      <c r="T23">
+      <c r="T23" s="4">
         <v>4</v>
       </c>
       <c r="U23">
@@ -1428,7 +1435,7 @@
       <c r="R26">
         <v>3</v>
       </c>
-      <c r="T26">
+      <c r="T26" s="4">
         <v>4</v>
       </c>
       <c r="U26">
@@ -1536,8 +1543,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="Q15:XFD20 O21:XFD21 O3:XFD6 A2:B6 O14:XFD14 Q7:XFD13 O28:XFD28 O22:P24 O25:Q27 V22:XFD27 A8:A11 C8:C11 A16:C16 C17:F18 O2:T2 V2:XFD2 O36:XFD1048576 Q35:XFD35 A21:B21 A19:F19 J2:L6 F2:H6 J20:L23 A24:L24 M2:M24 A7:L7 S23:T23 B20:C20 E20:H20 O33:XFD34 Q29:XFD32 B22:B23 B25:L32 A33:M1048576 A12:L12 F8:H11 J8:L11 A13:C13 C14:L15 F13:H13 J13:L13 G17:L19 J16:L16 F16:H16 T27 S26:T26 T24:T25 T22 E22:H23 F21:H21">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="1">
+  <conditionalFormatting sqref="Q15:XFD20 O21:XFD21 O3:XFD6 A2:B6 O14:XFD14 Q7:XFD13 O28:XFD28 O22:P24 O25:Q27 V22:XFD27 A8:A11 C8:C11 A16:C16 C17:F18 O2:T2 V2:XFD2 O36:XFD1048576 Q35:XFD35 A21:B21 A19:F19 J2:L6 F2:H6 J20:L23 A24:L24 M2:M24 A7:L7 S23 B20:C20 E20:H20 O33:XFD34 Q29:XFD32 B22:B23 B25:L32 A33:M1048576 A12:L12 F8:H11 J8:L11 A13:C13 C14:L15 F13:H13 J13:L13 G17:L19 J16:L16 F16:H16 T27 S26 T24:T25 T22 E22:H23 F21:H21">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
AbX, AbY addressing modes
</commit_message>
<xml_diff>
--- a/opcodes.xlsx
+++ b/opcodes.xlsx
@@ -308,7 +308,56 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1051,7 +1100,7 @@
       <c r="I8" s="4">
         <v>6</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="4">
         <v>7</v>
       </c>
       <c r="O8" s="3" t="s">
@@ -1077,7 +1126,7 @@
       <c r="I9" s="4">
         <v>6</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="4">
         <v>7</v>
       </c>
       <c r="O9" s="3" t="s">
@@ -1103,7 +1152,7 @@
       <c r="I10" s="4">
         <v>6</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="4">
         <v>7</v>
       </c>
       <c r="O10" s="3" t="s">
@@ -1129,7 +1178,7 @@
       <c r="I11" s="4">
         <v>6</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="4">
         <v>7</v>
       </c>
       <c r="O11" s="3" t="s">
@@ -1160,7 +1209,7 @@
       <c r="I13" s="4">
         <v>6</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="4">
         <v>7</v>
       </c>
       <c r="O13" s="3" t="s">
@@ -1205,7 +1254,7 @@
       <c r="I16" s="4">
         <v>6</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="4">
         <v>7</v>
       </c>
       <c r="O16" s="3" t="s">
@@ -1409,10 +1458,10 @@
       <c r="U25">
         <v>4</v>
       </c>
-      <c r="V25">
+      <c r="V25" s="4">
         <v>5</v>
       </c>
-      <c r="W25">
+      <c r="W25" s="4">
         <v>5</v>
       </c>
       <c r="Y25">
@@ -1543,8 +1592,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="Q15:XFD20 O21:XFD21 O3:XFD6 A2:B6 O14:XFD14 Q7:XFD13 O28:XFD28 O22:P24 O25:Q27 V22:XFD27 A8:A11 C8:C11 A16:C16 C17:F18 O2:T2 V2:XFD2 O36:XFD1048576 Q35:XFD35 A21:B21 A19:F19 J2:L6 F2:H6 J20:L23 A24:L24 M2:M24 A7:L7 S23 B20:C20 E20:H20 O33:XFD34 Q29:XFD32 B22:B23 B25:L32 A33:M1048576 A12:L12 F8:H11 J8:L11 A13:C13 C14:L15 F13:H13 J13:L13 G17:L19 J16:L16 F16:H16 T27 S26 T24:T25 T22 E22:H23 F21:H21">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="1">
+  <conditionalFormatting sqref="Q15:XFD20 O21:XFD21 O3:XFD6 A2:B6 O14:XFD14 Q7:XFD13 O28:XFD28 O22:P24 O25:Q27 A8:A11 C8:C11 A16:C16 C17:F18 O2:T2 V2:XFD2 O36:XFD1048576 Q35:XFD35 A21:B21 A19:F19 L2:L6 F2:H6 J20:L20 A24:L24 M2:M24 A7:L7 S23 B20:C20 E20:H20 O33:XFD34 Q29:XFD32 B22:B23 B25:L32 A33:M1048576 A12:L12 F8:H11 K8:L11 A13:C13 C14:L15 F13:H13 K13:L13 G17:L19 K16:L16 F16:H16 T27 S26 T24:T25 T22 E22:H23 F21:H21 V26:XFD27 W24:XFD24 V23 X22:XFD23 X25:XFD25 J22:L23 L21">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
IzY addressing mode, IzX now 1 cycle advancei from spec
</commit_message>
<xml_diff>
--- a/opcodes.xlsx
+++ b/opcodes.xlsx
@@ -308,112 +308,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -484,8 +379,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="6" name="Ink 5"/>
@@ -498,7 +393,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="6" name="Ink 5"/>
@@ -959,7 +854,7 @@
       <c r="E2" s="4">
         <v>4</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <v>6</v>
       </c>
       <c r="H2" s="1">
@@ -997,7 +892,7 @@
       <c r="E3" s="4">
         <v>4</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <v>6</v>
       </c>
       <c r="H3" s="1">
@@ -1032,7 +927,7 @@
       <c r="E4" s="4">
         <v>4</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>6</v>
       </c>
       <c r="H4" s="1">
@@ -1067,7 +962,7 @@
       <c r="E5" s="4">
         <v>4</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <v>6</v>
       </c>
       <c r="H5" s="1">
@@ -1102,7 +997,7 @@
       <c r="E6" s="4">
         <v>4</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="4">
         <v>6</v>
       </c>
       <c r="H6" s="1">
@@ -1372,7 +1267,7 @@
       <c r="E21" s="4">
         <v>4</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="4">
         <v>6</v>
       </c>
       <c r="H21" s="1">
@@ -1422,7 +1317,7 @@
       <c r="W22" s="1">
         <v>4</v>
       </c>
-      <c r="Y22">
+      <c r="Y22" s="4">
         <v>6</v>
       </c>
       <c r="Z22" s="1">
@@ -1506,10 +1401,10 @@
       <c r="W25" s="4">
         <v>5</v>
       </c>
-      <c r="Y25">
-        <v>6</v>
-      </c>
-      <c r="Z25">
+      <c r="Y25" s="4">
+        <v>6</v>
+      </c>
+      <c r="Z25" s="4">
         <v>6</v>
       </c>
     </row>
@@ -1634,8 +1529,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="Q15:XFD20 O21:XFD21 O3:XFD6 A2:B6 O14:XFD14 Q7:XFD13 O28:XFD28 O22:P22 O25:Q25 C8:C11 B16:C16 C17:F18 O2:T2 V2:XFD2 O36:XFD1048576 Q35:XFD35 A21:B21 A19:F19 L2:L6 F2:F6 J20:L20 A24:L24 M2:M24 A7:L7 S23 B20:C20 E20:H20 O33:XFD34 Q29:XFD32 B22:B23 B25:L32 A33:M1048576 A12:L12 F8:H11 K8:L11 B13:C13 C14:L15 F13:H13 K13:L13 G17:L19 K16:L16 F16:H16 T27 S26 T24:T25 T22 E22:H23 F21 V26:XFD27 W24:XFD24 V23 X23:XFD23 X25 J22:L23 L21 P26:Q27 P23:P24 H2:H6 H21 X22 Z22:XFD22 Z25:XFD25">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="1">
+  <conditionalFormatting sqref="Q15:XFD20 O21:XFD21 O3:XFD6 B2:B6 O14:XFD14 Q7:XFD13 O28:XFD28 C8:C11 B16:C16 C17:F18 O2:T2 V2:XFD2 O36:XFD1048576 Q35:XFD35 A19:F19 L2:L6 F2:F6 J20:L20 A24:L24 M2:M24 A7:L7 S23 B20:C20 E20:H20 O33:XFD34 Q29:XFD32 B21:B23 B25:L32 A33:M1048576 A12:L12 F8:H11 K8:L11 B13:C13 C14:L15 F13:H13 K13:L13 G17:L19 K16:L16 F16:H16 T27 S26 T24:T25 T22 E22:H23 F21 V26:XFD27 W24:XFD24 V23 X23:XFD23 X25 J22:L23 L21 P25:Q27 P22:P24 X22 AA22:XFD22 AA25:XFD25">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
RTS Return from stack
</commit_message>
<xml_diff>
--- a/opcodes.xlsx
+++ b/opcodes.xlsx
@@ -308,7 +308,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1543,8 +1550,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="Q15:XFD20 O21:XFD21 O4:XFD6 B2:B6 O14:XFD14 Q7:XFD13 O28:XFD28 C8:C11 B16:C16 C17:F18 V2:W2 O36:XFD1048576 Q35:XFD35 A19:F19 L2:L6 F2:F6 J20:L20 A24:L24 M2:M24 A7:L7 S23 B20:C20 E20:H20 O33:XFD34 Q29:XFD32 B21:B23 B25:L32 A33:M1048576 A12:L12 F8:H11 K8:L11 B13:C13 C14:L15 F13:H13 K13:L13 G17:L19 K16:L16 F16:H16 T27 S26 T24:T25 T22 E22:H23 F21 V26:XFD27 W24:XFD24 V23 X23:XFD23 X25 J22:L23 L21 P25:Q27 P22:P24 X22 AA22:XFD22 AA25:XFD25 Y2:XFD2 P2:T3 V3:XFD3">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="1">
+  <conditionalFormatting sqref="Q15:XFD20 O21:XFD21 O4:XFD4 B2:B6 O14:XFD14 Q7:XFD13 O28:XFD28 C8:C11 B16:C16 C17:F18 V2:W2 O36:XFD1048576 Q35:XFD35 A19:F19 L2:L6 F2:F6 J20:L20 A24:L24 M2:M24 A7:L7 S23 B20:C20 E20:H20 O33:XFD34 Q29:XFD32 B21:B23 B25:L32 A33:M1048576 A12:L12 F8:H11 K8:L11 B13:C13 C14:L15 F13:H13 K13:L13 G17:L19 K16:L16 F16:H16 T27 S26 T24:T25 T22 E22:H23 F21 V26:XFD27 W24:XFD24 V23 X23:XFD23 X25 J22:L23 L21 P25:Q27 P22:P24 X22 AA22:XFD22 AA25:XFD25 Y2:XFD2 P2:T3 V3:XFD3 O6:XFD6 Q5:XFD5">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Synthesis fix, spreadsheet update
</commit_message>
<xml_diff>
--- a/opcodes.xlsx
+++ b/opcodes.xlsx
@@ -308,7 +308,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1494,8 +1501,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="Q15:XFD20 O21:XFD21 O4:XFD4 B2:B6 O14:XFD14 Q7:XFD13 O28:XFD28 C8:C11 B16:C16 C17:F18 V2:W2 O36:XFD1048576 Q35:XFD35 A19:F19 L2:L6 F2:F6 J20:L20 A24:L24 M2:M24 A7:L7 S23 B20:C20 E20:H20 O33:XFD34 Q29:XFD32 B21:B23 B25:L32 A33:M1048576 A12:L12 F8:H11 K8:L11 B13:C13 C14:L15 F13:H13 K13:L13 G17:L19 K16:L16 F16:H16 T27 S26 T24:T25 T22 E22:H23 F21 V26:XFD27 W24:XFD24 V23 X23:XFD23 X25 J22:L23 L21 P25:Q27 P22:P24 X22 AA22:XFD22 AA25:XFD25 Y2:XFD2 P2:T3 V3:XFD3 O6:XFD6 Q5:XFD5">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+  <conditionalFormatting sqref="Q15:XFD20 O21:XFD21 O4:XFD4 B2:B6 O14:XFD14 Q7:XFD13 O28:XFD28 C8:C11 B16:C16 C17:F18 V2:W2 O36:XFD1048576 A19:F19 L2:L6 F2:F6 J20:L20 A24:L24 M2:M24 A7:L7 S23 B20:C20 E20:H20 O33:XFD33 Q29:XFD32 B21:B23 B25:L32 A33:M1048576 A12:L12 F8:H11 K8:L11 B13:C13 C14:L15 F13:H13 K13:L13 G17:L19 K16:L16 F16:H16 T27 S26 T24:T25 T22 E22:H23 F21 V26:XFD27 W24:XFD24 V23 X23:XFD23 X25 J22:L23 L21 P25:Q27 P22:P24 X22 AA22:XFD22 AA25:XFD25 Y2:XFD2 P2:T3 V3:XFD3 O6:XFD6 Q5:XFD5 Q34:XFD35">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>